<commit_message>
Notes from class on November 26, 2019
</commit_message>
<xml_diff>
--- a/FinalProject/Data/DataClean/SOC5800_Data_QualitativeAnalysis.xlsx
+++ b/FinalProject/Data/DataClean/SOC5800_Data_QualitativeAnalysis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="698" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="698" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Q38" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1832" uniqueCount="326">
   <si>
     <t>responseID</t>
   </si>
@@ -1039,6 +1039,12 @@
   </si>
   <si>
     <t>DF</t>
+  </si>
+  <si>
+    <t>NS</t>
+  </si>
+  <si>
+    <t>MT</t>
   </si>
 </sst>
 </file>
@@ -2953,7 +2959,7 @@
       </c>
       <c r="D1" s="12" t="str">
         <f>'Q41 Coder 2'!$C1</f>
-        <v>Coder 2</v>
+        <v>NS</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>264</v>
@@ -4850,7 +4856,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4868,7 +4874,7 @@
         <v>63</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>263</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5537,8 +5543,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8500,9 +8506,9 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9642,7 +9648,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9663,11 +9669,11 @@
       </c>
       <c r="C1" s="12" t="str">
         <f>'Q40 Coder 1'!$C1</f>
-        <v>Coder 1</v>
+        <v>DF</v>
       </c>
       <c r="D1" s="12" t="str">
         <f>'Q40 Coder 2'!$C1</f>
-        <v>Coder 2</v>
+        <v>MT</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>264</v>
@@ -10892,7 +10898,7 @@
         <v>62</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>262</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -11562,7 +11568,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11580,7 +11586,7 @@
         <v>62</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>263</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>